<commit_message>
implemented set_ranges(). Copy colors
</commit_message>
<xml_diff>
--- a/src/testTradingPost.xlsx
+++ b/src/testTradingPost.xlsx
@@ -655,7 +655,7 @@
       <u val="single"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="23">
     <fill>
       <patternFill/>
     </fill>
@@ -760,6 +760,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9E35D"/>
+        <bgColor rgb="FFF9E35D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FF92D050"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAD9507"/>
+        <bgColor rgb="FFAD9507"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="34">
     <border>
@@ -1171,7 +1195,7 @@
     </xf>
     <xf numFmtId="0" fontId="82" fillId="17" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="289">
+  <cellXfs count="299">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2037,6 +2061,36 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="18" fillId="19" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="67" fillId="20" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="20" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="67" fillId="21" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="67" fillId="19" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="19" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="67" fillId="19" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="67" fillId="22" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="20" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="21" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3207,13 +3261,41 @@
         </is>
       </c>
       <c r="B9" s="212" t="n"/>
-      <c r="C9" s="40" t="n"/>
-      <c r="D9" s="40" t="n"/>
-      <c r="E9" s="40" t="n"/>
-      <c r="F9" s="40" t="n"/>
-      <c r="G9" s="40" t="n"/>
-      <c r="H9" s="40" t="n"/>
-      <c r="I9" s="40" t="n"/>
+      <c r="C9" s="40" t="inlineStr">
+        <is>
+          <t>06/19</t>
+        </is>
+      </c>
+      <c r="D9" s="40" t="inlineStr">
+        <is>
+          <t>06/19</t>
+        </is>
+      </c>
+      <c r="E9" s="40" t="inlineStr">
+        <is>
+          <t>06/19</t>
+        </is>
+      </c>
+      <c r="F9" s="40" t="inlineStr">
+        <is>
+          <t>06/19</t>
+        </is>
+      </c>
+      <c r="G9" s="40" t="inlineStr">
+        <is>
+          <t>06/19</t>
+        </is>
+      </c>
+      <c r="H9" s="40" t="inlineStr">
+        <is>
+          <t>06/19</t>
+        </is>
+      </c>
+      <c r="I9" s="40" t="inlineStr">
+        <is>
+          <t>06/19</t>
+        </is>
+      </c>
       <c r="L9" s="230" t="inlineStr">
         <is>
           <t>Signal</t>
@@ -3299,33 +3381,40 @@
         </is>
       </c>
       <c r="B11" s="141" t="n"/>
-      <c r="C11" s="209">
-        <f>+[1]Sheet1!$R$6</f>
-        <v/>
-      </c>
-      <c r="D11" s="210">
-        <f>+[1]Sheet1!$R$7</f>
-        <v/>
-      </c>
-      <c r="E11" s="209">
-        <f>+[1]Sheet1!$N$8</f>
-        <v/>
-      </c>
-      <c r="F11" s="211">
-        <f>+[1]Sheet1!$N$9</f>
-        <v/>
-      </c>
-      <c r="G11" s="209">
-        <f>+[1]Sheet1!$R$11</f>
-        <v/>
-      </c>
-      <c r="H11" s="210">
-        <f>+[1]Sheet1!$R$12</f>
-        <v/>
-      </c>
-      <c r="I11" s="210">
-        <f>+[1]Sheet1!$R$13</f>
-        <v/>
+      <c r="C11" s="289" t="inlineStr">
+        <is>
+          <t>HOLD</t>
+        </is>
+      </c>
+      <c r="D11" s="290" t="inlineStr">
+        <is>
+          <t>HOLD</t>
+        </is>
+      </c>
+      <c r="E11" s="289" t="inlineStr">
+        <is>
+          <t>HOLD</t>
+        </is>
+      </c>
+      <c r="F11" s="291" t="inlineStr">
+        <is>
+          <t>HOLD</t>
+        </is>
+      </c>
+      <c r="G11" s="289" t="inlineStr">
+        <is>
+          <t>HOLD</t>
+        </is>
+      </c>
+      <c r="H11" s="292" t="inlineStr">
+        <is>
+          <t>HOLD</t>
+        </is>
+      </c>
+      <c r="I11" s="290" t="inlineStr">
+        <is>
+          <t>HOLD</t>
+        </is>
       </c>
       <c r="L11" s="230" t="inlineStr">
         <is>
@@ -3360,25 +3449,21 @@
         </is>
       </c>
       <c r="B12" s="140" t="n"/>
-      <c r="C12" s="78" t="n"/>
-      <c r="D12" s="78">
-        <f>+[1]Sheet1!$Z$7</f>
-        <v/>
-      </c>
-      <c r="E12" s="78" t="n"/>
-      <c r="F12" s="78">
-        <f>+[1]Sheet1!$X$9</f>
-        <v/>
-      </c>
-      <c r="G12" s="78" t="n"/>
-      <c r="H12" s="78">
-        <f>+[1]Sheet1!$Z$12</f>
-        <v/>
-      </c>
-      <c r="I12" s="78">
-        <f>+[1]Sheet1!$Z$13</f>
-        <v/>
-      </c>
+      <c r="C12" s="78" t="n">
+        <v>91.47</v>
+      </c>
+      <c r="D12" s="78" t="inlineStr"/>
+      <c r="E12" s="78" t="n">
+        <v>248.77</v>
+      </c>
+      <c r="F12" s="78" t="inlineStr"/>
+      <c r="G12" s="78" t="n">
+        <v>154.48</v>
+      </c>
+      <c r="H12" s="78" t="n">
+        <v>107.14</v>
+      </c>
+      <c r="I12" s="78" t="inlineStr"/>
       <c r="L12" s="273" t="inlineStr">
         <is>
           <t>Current</t>
@@ -3421,25 +3506,21 @@
         </is>
       </c>
       <c r="B13" s="140" t="n"/>
-      <c r="C13" s="79" t="n"/>
-      <c r="D13" s="79">
-        <f>+[1]Sheet1!$AA$7</f>
-        <v/>
-      </c>
-      <c r="E13" s="79" t="n"/>
-      <c r="F13" s="79">
-        <f>+[1]Sheet1!$Y$9</f>
-        <v/>
-      </c>
-      <c r="G13" s="79" t="n"/>
-      <c r="H13" s="79">
-        <f>+[1]Sheet1!$AA$12</f>
-        <v/>
-      </c>
-      <c r="I13" s="79">
-        <f>+[1]Sheet1!$AA$13</f>
-        <v/>
-      </c>
+      <c r="C13" s="79" t="n">
+        <v>91.37</v>
+      </c>
+      <c r="D13" s="79" t="inlineStr"/>
+      <c r="E13" s="79" t="n">
+        <v>251.95</v>
+      </c>
+      <c r="F13" s="79" t="inlineStr"/>
+      <c r="G13" s="79" t="n">
+        <v>153.27</v>
+      </c>
+      <c r="H13" s="79" t="n">
+        <v>112.94</v>
+      </c>
+      <c r="I13" s="79" t="inlineStr"/>
       <c r="L13" s="230" t="n"/>
       <c r="T13" s="86" t="n"/>
     </row>
@@ -3451,25 +3532,25 @@
       </c>
       <c r="B14" s="142" t="n"/>
       <c r="C14" s="120" t="n">
-        <v>91.67</v>
+        <v>91.91</v>
       </c>
       <c r="D14" s="81" t="n">
-        <v>30.89</v>
+        <v>31.39</v>
       </c>
       <c r="E14" s="82" t="n">
-        <v>276.76</v>
+        <v>277.3</v>
       </c>
       <c r="F14" s="81" t="n">
-        <v>192.71</v>
+        <v>195.57</v>
       </c>
       <c r="G14" s="83" t="n">
-        <v>159.48</v>
+        <v>161.25</v>
       </c>
       <c r="H14" s="80" t="n">
-        <v>112.09</v>
+        <v>112.24</v>
       </c>
       <c r="I14" s="82" t="n">
-        <v>80.8</v>
+        <v>81.2</v>
       </c>
       <c r="L14" s="235" t="inlineStr">
         <is>
@@ -3848,13 +3929,41 @@
     <row r="19" ht="24" customFormat="1" customHeight="1" s="1" thickBot="1">
       <c r="A19" s="18" t="n"/>
       <c r="B19" s="215" t="n"/>
-      <c r="C19" s="216" t="n"/>
-      <c r="D19" s="217" t="n"/>
-      <c r="E19" s="218" t="n"/>
-      <c r="F19" s="217" t="n"/>
-      <c r="G19" s="219" t="n"/>
-      <c r="H19" s="220" t="n"/>
-      <c r="I19" s="216" t="n"/>
+      <c r="C19" s="216" t="inlineStr">
+        <is>
+          <t>06/19</t>
+        </is>
+      </c>
+      <c r="D19" s="217" t="inlineStr">
+        <is>
+          <t>06/19</t>
+        </is>
+      </c>
+      <c r="E19" s="218" t="inlineStr">
+        <is>
+          <t>06/19</t>
+        </is>
+      </c>
+      <c r="F19" s="217" t="inlineStr">
+        <is>
+          <t>06/19</t>
+        </is>
+      </c>
+      <c r="G19" s="219" t="inlineStr">
+        <is>
+          <t>06/19</t>
+        </is>
+      </c>
+      <c r="H19" s="220" t="inlineStr">
+        <is>
+          <t>06/19</t>
+        </is>
+      </c>
+      <c r="I19" s="216" t="inlineStr">
+        <is>
+          <t>06/19</t>
+        </is>
+      </c>
       <c r="J19" s="281" t="n"/>
       <c r="K19" s="281" t="n"/>
       <c r="L19" s="230" t="inlineStr">
@@ -3960,33 +4069,40 @@
         </is>
       </c>
       <c r="B21" s="142" t="n"/>
-      <c r="C21" s="162">
-        <f>+[1]Sheet1!$R$14</f>
-        <v/>
-      </c>
-      <c r="D21" s="115">
-        <f>+[1]Sheet1!$R$16</f>
-        <v/>
-      </c>
-      <c r="E21" s="159">
-        <f>+[1]Sheet1!$R$17</f>
-        <v/>
-      </c>
-      <c r="F21" s="164">
-        <f>+[1]Sheet1!$R$18</f>
-        <v/>
-      </c>
-      <c r="G21" s="159">
-        <f>+[1]Sheet1!$R$19</f>
-        <v/>
-      </c>
-      <c r="H21" s="115">
-        <f>+[1]Sheet1!$N$21</f>
-        <v/>
-      </c>
-      <c r="I21" s="159">
-        <f>+[1]Sheet1!$R$22</f>
-        <v/>
+      <c r="C21" s="293" t="inlineStr">
+        <is>
+          <t>HOLD</t>
+        </is>
+      </c>
+      <c r="D21" s="294" t="inlineStr">
+        <is>
+          <t>HOLD</t>
+        </is>
+      </c>
+      <c r="E21" s="295" t="inlineStr">
+        <is>
+          <t>HOLD</t>
+        </is>
+      </c>
+      <c r="F21" s="296" t="inlineStr">
+        <is>
+          <t>!SELL!</t>
+        </is>
+      </c>
+      <c r="G21" s="295" t="inlineStr">
+        <is>
+          <t>HOLD</t>
+        </is>
+      </c>
+      <c r="H21" s="297" t="inlineStr">
+        <is>
+          <t>HOLD</t>
+        </is>
+      </c>
+      <c r="I21" s="295" t="inlineStr">
+        <is>
+          <t>HOLD</t>
+        </is>
       </c>
       <c r="J21" s="281" t="n"/>
       <c r="K21" s="281" t="n"/>
@@ -4017,27 +4133,24 @@
         </is>
       </c>
       <c r="B22" s="142" t="n"/>
-      <c r="C22" s="78">
-        <f>+[1]Sheet1!$Z$14</f>
-        <v/>
-      </c>
-      <c r="D22" s="78" t="n"/>
-      <c r="E22" s="78">
-        <f>+[1]Sheet1!$Z$17</f>
-        <v/>
-      </c>
-      <c r="F22" s="78">
-        <f>+[1]Sheet1!$Z$18</f>
-        <v/>
-      </c>
-      <c r="G22" s="78">
-        <f>+[1]Sheet1!$Z$19</f>
-        <v/>
-      </c>
-      <c r="H22" s="78" t="n"/>
-      <c r="I22" s="78">
-        <f>+[1]Sheet1!$Z$22</f>
-        <v/>
+      <c r="C22" s="78" t="n">
+        <v>40.05</v>
+      </c>
+      <c r="D22" s="78" t="n">
+        <v>242.07</v>
+      </c>
+      <c r="E22" s="78" t="n">
+        <v>187.18</v>
+      </c>
+      <c r="F22" s="78" t="n">
+        <v>384.65</v>
+      </c>
+      <c r="G22" s="78" t="n">
+        <v>173.58</v>
+      </c>
+      <c r="H22" s="78" t="inlineStr"/>
+      <c r="I22" s="78" t="n">
+        <v>376.75</v>
       </c>
       <c r="J22" s="281" t="n"/>
       <c r="K22" s="281" t="n"/>
@@ -4100,27 +4213,24 @@
         </is>
       </c>
       <c r="B23" s="142" t="n"/>
-      <c r="C23" s="79">
-        <f>+[1]Sheet1!$AA$14</f>
-        <v/>
-      </c>
-      <c r="D23" s="79" t="n"/>
-      <c r="E23" s="79">
-        <f>+[1]Sheet1!$AA$17</f>
-        <v/>
-      </c>
-      <c r="F23" s="79">
-        <f>+[1]Sheet1!$AA$18</f>
-        <v/>
-      </c>
-      <c r="G23" s="79">
-        <f>+[1]Sheet1!$AA$19</f>
-        <v/>
-      </c>
-      <c r="H23" s="79" t="n"/>
-      <c r="I23" s="79">
-        <f>+[1]Sheet1!$AA$22</f>
-        <v/>
+      <c r="C23" s="79" t="n">
+        <v>39.68</v>
+      </c>
+      <c r="D23" s="79" t="n">
+        <v>241.02</v>
+      </c>
+      <c r="E23" s="79" t="n">
+        <v>184.33</v>
+      </c>
+      <c r="F23" s="79" t="n">
+        <v>418.12</v>
+      </c>
+      <c r="G23" s="79" t="n">
+        <v>172.08</v>
+      </c>
+      <c r="H23" s="79" t="inlineStr"/>
+      <c r="I23" s="79" t="n">
+        <v>383.82</v>
       </c>
       <c r="J23" s="281" t="n"/>
       <c r="K23" s="281" t="n"/>
@@ -4188,25 +4298,25 @@
       </c>
       <c r="B24" s="142" t="n"/>
       <c r="C24" s="82" t="n">
-        <v>41.3</v>
+        <v>41.94</v>
       </c>
       <c r="D24" s="81" t="n">
-        <v>243.69</v>
+        <v>244.53</v>
       </c>
       <c r="E24" s="82" t="n">
-        <v>199.44</v>
+        <v>201.18</v>
       </c>
       <c r="F24" s="81" t="n">
-        <v>434.09</v>
+        <v>439.56</v>
       </c>
       <c r="G24" s="82" t="n">
-        <v>178.69</v>
+        <v>179.37</v>
       </c>
       <c r="H24" s="84" t="n">
-        <v>83.23</v>
+        <v>83.92</v>
       </c>
       <c r="I24" s="80" t="n">
-        <v>401.29</v>
+        <v>405.25</v>
       </c>
       <c r="J24" s="281" t="n"/>
       <c r="K24" s="281" t="n"/>
@@ -4533,13 +4643,41 @@
     <row r="29" ht="17" customHeight="1" s="288" thickBot="1">
       <c r="A29" s="33" t="n"/>
       <c r="B29" s="29" t="n"/>
-      <c r="C29" s="45" t="n"/>
-      <c r="D29" s="41" t="n"/>
-      <c r="E29" s="46" t="n"/>
-      <c r="F29" s="45" t="n"/>
-      <c r="G29" s="44" t="n"/>
-      <c r="H29" s="41" t="n"/>
-      <c r="I29" s="44" t="n"/>
+      <c r="C29" s="45" t="inlineStr">
+        <is>
+          <t>06/19</t>
+        </is>
+      </c>
+      <c r="D29" s="41" t="inlineStr">
+        <is>
+          <t>06/19</t>
+        </is>
+      </c>
+      <c r="E29" s="46" t="inlineStr">
+        <is>
+          <t>06/19</t>
+        </is>
+      </c>
+      <c r="F29" s="45" t="inlineStr">
+        <is>
+          <t>06/19</t>
+        </is>
+      </c>
+      <c r="G29" s="44" t="inlineStr">
+        <is>
+          <t>06/19</t>
+        </is>
+      </c>
+      <c r="H29" s="41" t="inlineStr">
+        <is>
+          <t>06/19</t>
+        </is>
+      </c>
+      <c r="I29" s="44" t="inlineStr">
+        <is>
+          <t>06/19</t>
+        </is>
+      </c>
       <c r="L29" s="232" t="n"/>
       <c r="P29" s="228" t="inlineStr">
         <is>
@@ -4583,33 +4721,40 @@
         </is>
       </c>
       <c r="B31" s="30" t="n"/>
-      <c r="C31" s="159">
-        <f>+[1]Sheet1!$R$23</f>
-        <v/>
-      </c>
-      <c r="D31" s="115">
-        <f>+[1]Sheet1!$R$24</f>
-        <v/>
-      </c>
-      <c r="E31" s="161">
-        <f>+[1]Sheet1!$N$26</f>
-        <v/>
-      </c>
-      <c r="F31" s="159">
-        <f>+[1]Sheet1!$R$27</f>
-        <v/>
-      </c>
-      <c r="G31" s="159">
-        <f>+[1]Sheet1!$R$28</f>
-        <v/>
-      </c>
-      <c r="H31" s="161">
-        <f>+[1]Sheet1!$N$29</f>
-        <v/>
-      </c>
-      <c r="I31" s="159">
-        <f>+[1]Sheet1!$R$30</f>
-        <v/>
+      <c r="C31" s="295" t="inlineStr">
+        <is>
+          <t>HOLD</t>
+        </is>
+      </c>
+      <c r="D31" s="297" t="inlineStr">
+        <is>
+          <t>HOLD</t>
+        </is>
+      </c>
+      <c r="E31" s="297" t="inlineStr">
+        <is>
+          <t>HOLD</t>
+        </is>
+      </c>
+      <c r="F31" s="295" t="inlineStr">
+        <is>
+          <t>HOLD</t>
+        </is>
+      </c>
+      <c r="G31" s="295" t="inlineStr">
+        <is>
+          <t>HOLD</t>
+        </is>
+      </c>
+      <c r="H31" s="298" t="inlineStr">
+        <is>
+          <t>HOLD</t>
+        </is>
+      </c>
+      <c r="I31" s="295" t="inlineStr">
+        <is>
+          <t>HOLD</t>
+        </is>
       </c>
       <c r="L31" s="253" t="inlineStr">
         <is>
@@ -4636,30 +4781,22 @@
         </is>
       </c>
       <c r="B32" s="28" t="n"/>
-      <c r="C32" s="78">
-        <f>+[1]Sheet1!$Z$23</f>
-        <v/>
-      </c>
-      <c r="D32" s="78" t="n"/>
-      <c r="E32" s="78">
-        <f>+[1]Sheet1!$X$26</f>
-        <v/>
-      </c>
-      <c r="F32" s="78">
-        <f>+[1]Sheet1!$Z$27</f>
-        <v/>
-      </c>
-      <c r="G32" s="78">
-        <f>+[1]Sheet1!$Z$28</f>
-        <v/>
-      </c>
-      <c r="H32" s="78">
-        <f>+[1]Sheet1!$X$29</f>
-        <v/>
-      </c>
-      <c r="I32" s="78">
-        <f>+[1]Sheet1!$Z$30</f>
-        <v/>
+      <c r="C32" s="78" t="n">
+        <v>97.40000000000001</v>
+      </c>
+      <c r="D32" s="78" t="inlineStr"/>
+      <c r="E32" s="78" t="inlineStr"/>
+      <c r="F32" s="78" t="n">
+        <v>55.51</v>
+      </c>
+      <c r="G32" s="78" t="n">
+        <v>203.78</v>
+      </c>
+      <c r="H32" s="78" t="n">
+        <v>141.59</v>
+      </c>
+      <c r="I32" s="78" t="n">
+        <v>72.20999999999999</v>
       </c>
       <c r="L32" s="254" t="inlineStr">
         <is>
@@ -4686,30 +4823,22 @@
         </is>
       </c>
       <c r="B33" s="28" t="n"/>
-      <c r="C33" s="79">
-        <f>+[1]Sheet1!$AA$23</f>
-        <v/>
-      </c>
-      <c r="D33" s="79" t="n"/>
-      <c r="E33" s="79">
-        <f>+[1]Sheet1!$Y$26</f>
-        <v/>
-      </c>
-      <c r="F33" s="79">
-        <f>+[1]Sheet1!$AA$27</f>
-        <v/>
-      </c>
-      <c r="G33" s="79">
-        <f>+[1]Sheet1!$AA$28</f>
-        <v/>
-      </c>
-      <c r="H33" s="79">
-        <f>+[1]Sheet1!$Y$29</f>
-        <v/>
-      </c>
-      <c r="I33" s="79">
-        <f>+[1]Sheet1!$AA$30</f>
-        <v/>
+      <c r="C33" s="79" t="n">
+        <v>101.35</v>
+      </c>
+      <c r="D33" s="79" t="inlineStr"/>
+      <c r="E33" s="79" t="inlineStr"/>
+      <c r="F33" s="79" t="n">
+        <v>54.11</v>
+      </c>
+      <c r="G33" s="79" t="n">
+        <v>207.12</v>
+      </c>
+      <c r="H33" s="79" t="n">
+        <v>147.24</v>
+      </c>
+      <c r="I33" s="79" t="n">
+        <v>71.98999999999999</v>
       </c>
       <c r="L33" s="255" t="inlineStr">
         <is>
@@ -4737,25 +4866,25 @@
       </c>
       <c r="B34" s="30" t="n"/>
       <c r="C34" s="96" t="n">
-        <v>105.32</v>
+        <v>106.2</v>
       </c>
       <c r="D34" s="98" t="n">
-        <v>72.38</v>
+        <v>72.73</v>
       </c>
       <c r="E34" s="99" t="n">
-        <v>48.57</v>
+        <v>48.64</v>
       </c>
       <c r="F34" s="96" t="n">
-        <v>57</v>
+        <v>57.62</v>
       </c>
       <c r="G34" s="98" t="n">
-        <v>217.44</v>
+        <v>219.26</v>
       </c>
       <c r="H34" s="100" t="n">
-        <v>144.2</v>
+        <v>146.24</v>
       </c>
       <c r="I34" s="98" t="n">
-        <v>78.804</v>
+        <v>79.92</v>
       </c>
       <c r="L34" s="260" t="n"/>
       <c r="M34" s="261" t="n"/>

</xml_diff>

<commit_message>
integrated generate_csv with etf object
</commit_message>
<xml_diff>
--- a/src/testTradingPost.xlsx
+++ b/src/testTradingPost.xlsx
@@ -486,8 +486,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="14"/>
-        <bgColor indexed="14"/>
+        <fgColor indexed="16"/>
+        <bgColor indexed="16"/>
       </patternFill>
     </fill>
   </fills>
@@ -3594,12 +3594,12 @@
       <c r="B8" s="67" t="n"/>
       <c r="C8" s="68" t="inlineStr">
         <is>
-          <t>Hi. Yield</t>
+          <t>name</t>
         </is>
       </c>
       <c r="D8" s="68" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>Gold</t>
         </is>
       </c>
       <c r="E8" s="68" t="inlineStr">
@@ -3718,12 +3718,12 @@
       <c r="B10" s="238" t="n"/>
       <c r="C10" s="76" t="inlineStr">
         <is>
+          <t>06/25</t>
+        </is>
+      </c>
+      <c r="D10" s="76" t="inlineStr">
+        <is>
           <t>06/02</t>
-        </is>
-      </c>
-      <c r="D10" s="76" t="inlineStr">
-        <is>
-          <t>06/25</t>
         </is>
       </c>
       <c r="E10" s="76" t="inlineStr">
@@ -3844,12 +3844,12 @@
         </is>
       </c>
       <c r="B12" s="239" t="n"/>
-      <c r="C12" s="79" t="inlineStr">
+      <c r="C12" s="240" t="inlineStr">
         <is>
           <t>HOLD</t>
         </is>
       </c>
-      <c r="D12" s="240" t="inlineStr">
+      <c r="D12" s="79" t="inlineStr">
         <is>
           <t>HOLD</t>
         </is>
@@ -3908,10 +3908,10 @@
         </is>
       </c>
       <c r="B13" s="71" t="n"/>
-      <c r="C13" s="241" t="n"/>
-      <c r="D13" s="241" t="n">
-        <v>29.29</v>
-      </c>
+      <c r="C13" s="241" t="n">
+        <v>90.86999999999999</v>
+      </c>
+      <c r="D13" s="241" t="n"/>
       <c r="E13" s="241" t="n">
         <v>249.41</v>
       </c>
@@ -3952,10 +3952,10 @@
         </is>
       </c>
       <c r="B14" s="71" t="n"/>
-      <c r="C14" s="242" t="n"/>
-      <c r="D14" s="242" t="n">
-        <v>32.65</v>
-      </c>
+      <c r="C14" s="242" t="n">
+        <v>90.89</v>
+      </c>
+      <c r="D14" s="242" t="n"/>
       <c r="E14" s="242" t="n">
         <v>257.15</v>
       </c>
@@ -3997,10 +3997,10 @@
       </c>
       <c r="B15" s="243" t="n"/>
       <c r="C15" s="244" t="n">
-        <v>91.38</v>
+        <v>90.90000000000001</v>
       </c>
       <c r="D15" s="245" t="n">
-        <v>29.79</v>
+        <v>31.41</v>
       </c>
       <c r="E15" s="245" t="n">
         <v>263.01</v>

</xml_diff>